<commit_message>
feat: initial rc for bff int
BREAKING CHANGES: Dynamic menus and api proxy
</commit_message>
<xml_diff>
--- a/AdHOCInvoiceApp/AdHOCInvoicingApp/ClientApp/src/assets/GRA_INVOICER_ITEMS_TEMPLATE.xlsx
+++ b/AdHOCInvoiceApp/AdHOCInvoicingApp/ClientApp/src/assets/GRA_INVOICER_ITEMS_TEMPLATE.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAMPOFO\Desktop\Me\ReactJS\gra-invoicer\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabila\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F7CCA94E-EC4E-48BE-993C-A601D3F14F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7E625F7-7C16-411A-8CE1-886F2BBAC022}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7290" windowHeight="3045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4740" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Wholesale Items List" sheetId="1" r:id="rId1"/>
-    <sheet name="Foreign Goods" sheetId="3" r:id="rId2"/>
+    <sheet name="Items" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ItemName</t>
   </si>
@@ -36,37 +47,46 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>5kg bag of rice</t>
-  </si>
-  <si>
     <t>Taxable</t>
   </si>
   <si>
+    <t>VATInclusive</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>CST/Toursim</t>
+  </si>
+  <si>
+    <t>Playstation 5</t>
+  </si>
+  <si>
+    <t>Game console</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Sugar</t>
-  </si>
-  <si>
-    <t>white sugar</t>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>Orthopedic Mattress</t>
+  </si>
+  <si>
+    <t>Queen sized mattress</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Playstation 5</t>
-  </si>
-  <si>
-    <t>Game console</t>
-  </si>
-  <si>
-    <t>Orthopedic Mattress</t>
-  </si>
-  <si>
-    <t>Queen sized mattress</t>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>TOUR</t>
   </si>
   <si>
     <t>Moped Bike</t>
@@ -75,47 +95,17 @@
     <t>Bike</t>
   </si>
   <si>
-    <t>VATInclusive</t>
-  </si>
-  <si>
-    <t>Gari</t>
-  </si>
-  <si>
-    <t>olonka</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>CST/Toursim</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>GHS</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>NON</t>
-  </si>
-  <si>
-    <t>TOUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,9 +114,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,17 +139,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,131 +426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>85</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>15.5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -572,53 +444,53 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>5000</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -629,42 +501,53 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>25000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1136 E1 D1:D1048576" xr:uid="{26D82B0A-E6A5-40B4-BB6B-86CFC779AD1E}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{880086C2-F058-4209-BF69-8020E67B2073}">
+      <formula1>"GHS, EUR, USD, GBP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{1A363835-FE9E-4A88-8237-6DE330DE3598}">
+      <formula1>"CST, TOUR, NON"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: changed the template files
</commit_message>
<xml_diff>
--- a/AdHOCInvoiceApp/AdHOCInvoicingApp/ClientApp/src/assets/GRA_INVOICER_ITEMS_TEMPLATE.xlsx
+++ b/AdHOCInvoiceApp/AdHOCInvoicingApp/ClientApp/src/assets/GRA_INVOICER_ITEMS_TEMPLATE.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26809"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabila\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hquaye\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F7CCA94E-EC4E-48BE-993C-A601D3F14F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7E625F7-7C16-411A-8CE1-886F2BBAC022}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC34666D-B405-45BB-BF08-0D792B71C28E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4740" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" xr2:uid="{227CD45E-BF51-4714-8FAE-349719B85EAA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="3" r:id="rId1"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>ItemName</t>
   </si>
@@ -59,54 +49,101 @@
     <t>CST/Toursim</t>
   </si>
   <si>
-    <t>Playstation 5</t>
-  </si>
-  <si>
-    <t>Game console</t>
+    <t>Macbook Pro</t>
+  </si>
+  <si>
+    <t>The MacBook Pro is a line of Mac laptops made by Apple Inc.</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Value Example</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Name of Item</t>
+  </si>
+  <si>
+    <t>Price of item</t>
+  </si>
+  <si>
+    <t>Description of item</t>
+  </si>
+  <si>
+    <t>CST/Tourism</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Does the item fall under Communication Service Tax (CST) or Tourism (TSRM) or None (NON). If left empty it defaults to NON</t>
+  </si>
+  <si>
+    <t>Is the item VATInclusive? If left empty it defaults to No</t>
+  </si>
+  <si>
+    <t>Is the item Taxable? If left empty it defaults to No</t>
+  </si>
+  <si>
+    <t>Currency in which item was bought. Can be either GHS, EUR, USD, GBP</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>CST/TOURISM</t>
+  </si>
+  <si>
+    <t>GHS</t>
+  </si>
+  <si>
     <t>EUR</t>
   </si>
   <si>
+    <t>GBP</t>
+  </si>
+  <si>
     <t>CST</t>
   </si>
   <si>
-    <t>Orthopedic Mattress</t>
-  </si>
-  <si>
-    <t>Queen sized mattress</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>TOUR</t>
-  </si>
-  <si>
-    <t>Moped Bike</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>NON</t>
+    <t>TSRM</t>
+  </si>
+  <si>
+    <t>YES/NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,16 +158,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -138,15 +198,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +289,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -193,7 +301,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -210,9 +318,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -240,14 +348,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -275,6 +400,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,129 +568,298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD960A89-D18D-4962-ACAD-F97A08EC6940}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>5000</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>3000</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>25000</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1136 E1 D1:D1048576" xr:uid="{26D82B0A-E6A5-40B4-BB6B-86CFC779AD1E}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{880086C2-F058-4209-BF69-8020E67B2073}">
-      <formula1>"GHS, EUR, USD, GBP"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{1A363835-FE9E-4A88-8237-6DE330DE3598}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{EC3425BB-0FD7-4A7B-85FB-387D75824F9F}">
       <formula1>"CST, TOUR, NON"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{880A5732-E2D3-4A1F-A022-833B7A8486D6}">
+          <x14:formula1>
+            <xm:f>Legend!$K$3:$K$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576 D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEE0A505-8802-4CAB-9217-8FD49CB0A816}">
+          <x14:formula1>
+            <xm:f>Legend!$H$3:$H$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1726BA7B-8888-4C96-8D7B-A1DAD9A1B5CE}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7">
+        <v>10000</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A13"/>
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>